<commit_message>
Iteration 3 Docs added.
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/Team_2_Iteration 2_Submission/Increment Matrix.xlsx
+++ b/Iteration 2 docs/Team_2_Iteration 2_Submission/Increment Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS 2020\ArlingtonAuto\Iteration 2 docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS 2020\ArlingtonAuto\Iteration 2 docs\Team_2_Iteration 2_Submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C74205-FBB0-4F47-89E3-5D4EFFB542D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E8221C-C092-4C47-834B-2EDAB4068099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Use Case Name</t>
   </si>
@@ -154,10 +154,23 @@
     <t>Iteration 2* (10/29/20)</t>
   </si>
   <si>
-    <t xml:space="preserve">Iteration 3* </t>
-  </si>
-  <si>
     <t>Search for Cars</t>
+  </si>
+  <si>
+    <t>Iteration 3* 
+(11/03/20)</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>EUC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>1(SD)</t>
   </si>
 </sst>
 </file>
@@ -195,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -218,16 +231,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -568,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +612,7 @@
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -593,22 +623,30 @@
         <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -619,8 +657,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -631,8 +671,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -643,8 +685,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -655,8 +699,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -667,8 +713,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -679,20 +727,24 @@
         <v>1</v>
       </c>
       <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2">
-        <v>1</v>
+      <c r="C9" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -703,8 +755,14 @@
       <c r="D10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -715,8 +773,11 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -727,8 +788,12 @@
       <c r="D12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -739,8 +804,12 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -751,8 +820,10 @@
         <v>1</v>
       </c>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -763,8 +834,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="4"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -775,8 +848,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -787,8 +862,12 @@
       <c r="D17" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -799,8 +878,12 @@
       <c r="D18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -811,8 +894,12 @@
       <c r="D19" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -823,20 +910,24 @@
         <v>1</v>
       </c>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
       </c>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -847,6 +938,8 @@
         <v>1</v>
       </c>
       <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>